<commit_message>
finish chart-5; init chart-6; rename
</commit_message>
<xml_diff>
--- a/408/计算机网络/assets/demo.xlsx
+++ b/408/计算机网络/assets/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\考研\408\计算机网络\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885D55C0-9DFF-4351-A1F8-7CB70F680285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDC1E54-BFA6-4CEC-A539-0B4CDDAE7F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>应用程序</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -199,12 +199,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -219,9 +237,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -504,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D14"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -522,206 +552,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="2">
         <v>21</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="2">
         <v>23</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="2">
         <v>25</v>
       </c>
-      <c r="E3" s="1">
-        <v>53</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1">
-        <v>69</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="E4" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="F4" s="2">
+        <v>110</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1">
-        <v>110</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B9" s="3">
+        <v>53</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3">
+        <v>69</v>
+      </c>
+      <c r="E9" s="3">
         <v>123</v>
       </c>
-      <c r="D7" s="1">
+      <c r="F9" s="3">
         <v>161</v>
       </c>
-      <c r="E7" s="1">
+      <c r="G9" s="3">
         <v>520</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>